<commit_message>
6 monthly coverage scenario 2 and 3a
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_2.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\ntd-model-sch\sch_simulation\data\SCH_params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD2C0D-D3AF-4A78-9B9A-0438946481FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301FE17B-43E3-4FD6-96B1-FBE1FEF4DEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AZ8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
     <col min="6" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,73 +489,139 @@
         <v>2018</v>
       </c>
       <c r="I1">
+        <v>2018.5</v>
+      </c>
+      <c r="J1">
         <v>2019</v>
       </c>
-      <c r="J1">
+      <c r="K1">
+        <v>2019.5</v>
+      </c>
+      <c r="L1">
         <v>2020</v>
       </c>
-      <c r="K1">
+      <c r="M1">
+        <v>2020.5</v>
+      </c>
+      <c r="N1">
         <v>2021</v>
       </c>
-      <c r="L1">
+      <c r="O1">
+        <v>2021.5</v>
+      </c>
+      <c r="P1">
         <v>2022</v>
       </c>
-      <c r="M1">
+      <c r="Q1">
+        <v>2022.5</v>
+      </c>
+      <c r="R1">
         <v>2023</v>
       </c>
-      <c r="N1">
+      <c r="S1">
+        <v>2023.5</v>
+      </c>
+      <c r="T1">
         <v>2024</v>
       </c>
-      <c r="O1">
+      <c r="U1">
+        <v>2024.5</v>
+      </c>
+      <c r="V1">
         <v>2025</v>
       </c>
-      <c r="P1">
+      <c r="W1">
+        <v>2025.5</v>
+      </c>
+      <c r="X1">
         <v>2026</v>
       </c>
-      <c r="Q1">
+      <c r="Y1">
+        <v>2026.5</v>
+      </c>
+      <c r="Z1">
         <v>2027</v>
       </c>
-      <c r="R1">
+      <c r="AA1">
+        <v>2027.5</v>
+      </c>
+      <c r="AB1">
         <v>2028</v>
       </c>
-      <c r="S1">
+      <c r="AC1">
+        <v>2028.5</v>
+      </c>
+      <c r="AD1">
         <v>2029</v>
       </c>
-      <c r="T1">
+      <c r="AE1">
+        <v>2029.5</v>
+      </c>
+      <c r="AF1">
         <v>2030</v>
       </c>
-      <c r="U1">
+      <c r="AG1">
+        <v>2030.5</v>
+      </c>
+      <c r="AH1">
         <v>2031</v>
       </c>
-      <c r="V1">
+      <c r="AI1">
+        <v>2031.5</v>
+      </c>
+      <c r="AJ1">
         <v>2032</v>
       </c>
-      <c r="W1">
+      <c r="AK1">
+        <v>2032.5</v>
+      </c>
+      <c r="AL1">
         <v>2033</v>
       </c>
-      <c r="X1">
+      <c r="AM1">
+        <v>2033.5</v>
+      </c>
+      <c r="AN1">
         <v>2034</v>
       </c>
-      <c r="Y1">
+      <c r="AO1">
+        <v>2034.5</v>
+      </c>
+      <c r="AP1">
         <v>2035</v>
       </c>
-      <c r="Z1">
+      <c r="AQ1">
+        <v>2035.5</v>
+      </c>
+      <c r="AR1">
         <v>2036</v>
       </c>
-      <c r="AA1">
+      <c r="AS1">
+        <v>2036.5</v>
+      </c>
+      <c r="AT1">
         <v>2037</v>
       </c>
-      <c r="AB1">
+      <c r="AU1">
+        <v>2037.5</v>
+      </c>
+      <c r="AV1">
         <v>2038</v>
       </c>
-      <c r="AC1">
+      <c r="AW1">
+        <v>2038.5</v>
+      </c>
+      <c r="AX1">
         <v>2039</v>
       </c>
-      <c r="AD1">
+      <c r="AY1">
+        <v>2039.5</v>
+      </c>
+      <c r="AZ1">
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -586,8 +652,20 @@
       <c r="N2">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>0.6</v>
+      </c>
+      <c r="R2">
+        <v>0.6</v>
+      </c>
+      <c r="T2">
+        <v>0.6</v>
+      </c>
+      <c r="V2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -606,32 +684,95 @@
       <c r="G3">
         <v>15</v>
       </c>
-      <c r="P3">
-        <v>0.75</v>
-      </c>
-      <c r="R3">
-        <v>0.75</v>
-      </c>
-      <c r="T3">
-        <v>0.75</v>
-      </c>
-      <c r="V3">
-        <v>0.75</v>
-      </c>
       <c r="X3">
         <v>0.75</v>
       </c>
+      <c r="Y3">
+        <v>0.75</v>
+      </c>
       <c r="Z3">
         <v>0.75</v>
       </c>
+      <c r="AA3">
+        <v>0.75</v>
+      </c>
       <c r="AB3">
         <v>0.75</v>
       </c>
+      <c r="AC3">
+        <v>0.75</v>
+      </c>
       <c r="AD3">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE3">
+        <v>0.75</v>
+      </c>
+      <c r="AF3">
+        <v>0.75</v>
+      </c>
+      <c r="AG3">
+        <v>0.75</v>
+      </c>
+      <c r="AH3">
+        <v>0.75</v>
+      </c>
+      <c r="AI3">
+        <v>0.75</v>
+      </c>
+      <c r="AJ3">
+        <v>0.75</v>
+      </c>
+      <c r="AK3">
+        <v>0.75</v>
+      </c>
+      <c r="AL3">
+        <v>0.75</v>
+      </c>
+      <c r="AM3">
+        <v>0.75</v>
+      </c>
+      <c r="AN3">
+        <v>0.75</v>
+      </c>
+      <c r="AO3">
+        <v>0.75</v>
+      </c>
+      <c r="AP3">
+        <v>0.75</v>
+      </c>
+      <c r="AQ3">
+        <v>0.75</v>
+      </c>
+      <c r="AR3">
+        <v>0.75</v>
+      </c>
+      <c r="AS3">
+        <v>0.75</v>
+      </c>
+      <c r="AT3">
+        <v>0.75</v>
+      </c>
+      <c r="AU3">
+        <v>0.75</v>
+      </c>
+      <c r="AV3">
+        <v>0.75</v>
+      </c>
+      <c r="AW3">
+        <v>0.75</v>
+      </c>
+      <c r="AX3">
+        <v>0.75</v>
+      </c>
+      <c r="AY3">
+        <v>0.75</v>
+      </c>
+      <c r="AZ3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -650,32 +791,95 @@
       <c r="G4">
         <v>50</v>
       </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="R4">
-        <v>0.5</v>
-      </c>
-      <c r="T4">
-        <v>0.5</v>
-      </c>
-      <c r="V4">
-        <v>0.5</v>
-      </c>
       <c r="X4">
         <v>0.5</v>
       </c>
+      <c r="Y4">
+        <v>0.5</v>
+      </c>
       <c r="Z4">
         <v>0.5</v>
       </c>
+      <c r="AA4">
+        <v>0.5</v>
+      </c>
       <c r="AB4">
         <v>0.5</v>
       </c>
+      <c r="AC4">
+        <v>0.5</v>
+      </c>
       <c r="AD4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE4">
+        <v>0.5</v>
+      </c>
+      <c r="AF4">
+        <v>0.5</v>
+      </c>
+      <c r="AG4">
+        <v>0.5</v>
+      </c>
+      <c r="AH4">
+        <v>0.5</v>
+      </c>
+      <c r="AI4">
+        <v>0.5</v>
+      </c>
+      <c r="AJ4">
+        <v>0.5</v>
+      </c>
+      <c r="AK4">
+        <v>0.5</v>
+      </c>
+      <c r="AL4">
+        <v>0.5</v>
+      </c>
+      <c r="AM4">
+        <v>0.5</v>
+      </c>
+      <c r="AN4">
+        <v>0.5</v>
+      </c>
+      <c r="AO4">
+        <v>0.5</v>
+      </c>
+      <c r="AP4">
+        <v>0.5</v>
+      </c>
+      <c r="AQ4">
+        <v>0.5</v>
+      </c>
+      <c r="AR4">
+        <v>0.5</v>
+      </c>
+      <c r="AS4">
+        <v>0.5</v>
+      </c>
+      <c r="AT4">
+        <v>0.5</v>
+      </c>
+      <c r="AU4">
+        <v>0.5</v>
+      </c>
+      <c r="AV4">
+        <v>0.5</v>
+      </c>
+      <c r="AW4">
+        <v>0.5</v>
+      </c>
+      <c r="AX4">
+        <v>0.5</v>
+      </c>
+      <c r="AY4">
+        <v>0.5</v>
+      </c>
+      <c r="AZ4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -694,32 +898,95 @@
       <c r="G5">
         <v>65</v>
       </c>
-      <c r="P5">
-        <v>0.5</v>
-      </c>
-      <c r="R5">
-        <v>0.5</v>
-      </c>
-      <c r="T5">
-        <v>0.5</v>
-      </c>
-      <c r="V5">
-        <v>0.5</v>
-      </c>
       <c r="X5">
         <v>0.5</v>
       </c>
+      <c r="Y5">
+        <v>0.5</v>
+      </c>
       <c r="Z5">
         <v>0.5</v>
       </c>
+      <c r="AA5">
+        <v>0.5</v>
+      </c>
       <c r="AB5">
         <v>0.5</v>
       </c>
+      <c r="AC5">
+        <v>0.5</v>
+      </c>
       <c r="AD5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE5">
+        <v>0.5</v>
+      </c>
+      <c r="AF5">
+        <v>0.5</v>
+      </c>
+      <c r="AG5">
+        <v>0.5</v>
+      </c>
+      <c r="AH5">
+        <v>0.5</v>
+      </c>
+      <c r="AI5">
+        <v>0.5</v>
+      </c>
+      <c r="AJ5">
+        <v>0.5</v>
+      </c>
+      <c r="AK5">
+        <v>0.5</v>
+      </c>
+      <c r="AL5">
+        <v>0.5</v>
+      </c>
+      <c r="AM5">
+        <v>0.5</v>
+      </c>
+      <c r="AN5">
+        <v>0.5</v>
+      </c>
+      <c r="AO5">
+        <v>0.5</v>
+      </c>
+      <c r="AP5">
+        <v>0.5</v>
+      </c>
+      <c r="AQ5">
+        <v>0.5</v>
+      </c>
+      <c r="AR5">
+        <v>0.5</v>
+      </c>
+      <c r="AS5">
+        <v>0.5</v>
+      </c>
+      <c r="AT5">
+        <v>0.5</v>
+      </c>
+      <c r="AU5">
+        <v>0.5</v>
+      </c>
+      <c r="AV5">
+        <v>0.5</v>
+      </c>
+      <c r="AW5">
+        <v>0.5</v>
+      </c>
+      <c r="AX5">
+        <v>0.5</v>
+      </c>
+      <c r="AY5">
+        <v>0.5</v>
+      </c>
+      <c r="AZ5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -739,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -759,7 +1026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1040,9 +1307,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1263,19 +1533,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1300,9 +1566,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add scenario files for runs march 8th 2023
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_2.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\ntd-model-sch\sch_simulation\data\SCH_params\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewgraham/Dropbox/ntd-model-sch/sch_simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301FE17B-43E3-4FD6-96B1-FBE1FEF4DEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4614FE51-E5EB-954C-8321-F2037B81E34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44020" windowHeight="20360" activeTab="1" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
   <sheets>
     <sheet name="Platform Coverage" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>Country/Region</t>
   </si>
@@ -96,16 +96,26 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Vector Control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,22 +459,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
-  <dimension ref="A1:AZ8"/>
+  <dimension ref="A1:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3:AZ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +632,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -640,32 +651,29 @@
       <c r="G2">
         <v>15</v>
       </c>
-      <c r="H2">
-        <v>0.6</v>
-      </c>
       <c r="J2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="L2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="N2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="P2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="R2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="T2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="V2">
-        <v>0.6</v>
+        <v>0.73599999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -685,94 +693,94 @@
         <v>15</v>
       </c>
       <c r="X3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="Y3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="Z3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AA3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AB3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AC3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AD3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AE3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AF3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AG3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AH3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AI3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AJ3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AK3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AL3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AM3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AN3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AO3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AP3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AQ3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AR3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AS3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AT3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AU3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AV3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AW3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AX3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AY3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AZ3">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -791,95 +799,95 @@
       <c r="G4">
         <v>50</v>
       </c>
-      <c r="X4">
-        <v>0.5</v>
-      </c>
-      <c r="Y4">
-        <v>0.5</v>
-      </c>
-      <c r="Z4">
-        <v>0.5</v>
-      </c>
-      <c r="AA4">
-        <v>0.5</v>
-      </c>
-      <c r="AB4">
-        <v>0.5</v>
-      </c>
-      <c r="AC4">
-        <v>0.5</v>
-      </c>
-      <c r="AD4">
-        <v>0.5</v>
-      </c>
-      <c r="AE4">
-        <v>0.5</v>
-      </c>
-      <c r="AF4">
-        <v>0.5</v>
-      </c>
-      <c r="AG4">
-        <v>0.5</v>
-      </c>
-      <c r="AH4">
-        <v>0.5</v>
-      </c>
-      <c r="AI4">
-        <v>0.5</v>
-      </c>
-      <c r="AJ4">
-        <v>0.5</v>
-      </c>
-      <c r="AK4">
-        <v>0.5</v>
-      </c>
-      <c r="AL4">
-        <v>0.5</v>
-      </c>
-      <c r="AM4">
-        <v>0.5</v>
-      </c>
-      <c r="AN4">
-        <v>0.5</v>
-      </c>
-      <c r="AO4">
-        <v>0.5</v>
-      </c>
-      <c r="AP4">
-        <v>0.5</v>
-      </c>
-      <c r="AQ4">
-        <v>0.5</v>
-      </c>
-      <c r="AR4">
-        <v>0.5</v>
-      </c>
-      <c r="AS4">
-        <v>0.5</v>
-      </c>
-      <c r="AT4">
-        <v>0.5</v>
-      </c>
-      <c r="AU4">
-        <v>0.5</v>
-      </c>
-      <c r="AV4">
-        <v>0.5</v>
-      </c>
-      <c r="AW4">
-        <v>0.5</v>
-      </c>
-      <c r="AX4">
-        <v>0.5</v>
-      </c>
-      <c r="AY4">
-        <v>0.5</v>
-      </c>
-      <c r="AZ4">
-        <v>0.5</v>
+      <c r="X4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AO4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AS4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AT4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AU4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AV4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AW4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AX4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AY4" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AZ4" s="2">
+        <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -898,95 +906,95 @@
       <c r="G5">
         <v>65</v>
       </c>
-      <c r="X5">
-        <v>0.5</v>
-      </c>
-      <c r="Y5">
-        <v>0.5</v>
-      </c>
-      <c r="Z5">
-        <v>0.5</v>
-      </c>
-      <c r="AA5">
-        <v>0.5</v>
-      </c>
-      <c r="AB5">
-        <v>0.5</v>
-      </c>
-      <c r="AC5">
-        <v>0.5</v>
-      </c>
-      <c r="AD5">
-        <v>0.5</v>
-      </c>
-      <c r="AE5">
-        <v>0.5</v>
-      </c>
-      <c r="AF5">
-        <v>0.5</v>
-      </c>
-      <c r="AG5">
-        <v>0.5</v>
-      </c>
-      <c r="AH5">
-        <v>0.5</v>
-      </c>
-      <c r="AI5">
-        <v>0.5</v>
-      </c>
-      <c r="AJ5">
-        <v>0.5</v>
-      </c>
-      <c r="AK5">
-        <v>0.5</v>
-      </c>
-      <c r="AL5">
-        <v>0.5</v>
-      </c>
-      <c r="AM5">
-        <v>0.5</v>
-      </c>
-      <c r="AN5">
-        <v>0.5</v>
-      </c>
-      <c r="AO5">
-        <v>0.5</v>
-      </c>
-      <c r="AP5">
-        <v>0.5</v>
-      </c>
-      <c r="AQ5">
-        <v>0.5</v>
-      </c>
-      <c r="AR5">
-        <v>0.5</v>
-      </c>
-      <c r="AS5">
-        <v>0.5</v>
-      </c>
-      <c r="AT5">
-        <v>0.5</v>
-      </c>
-      <c r="AU5">
-        <v>0.5</v>
-      </c>
-      <c r="AV5">
-        <v>0.5</v>
-      </c>
-      <c r="AW5">
-        <v>0.5</v>
-      </c>
-      <c r="AX5">
-        <v>0.5</v>
-      </c>
-      <c r="AY5">
-        <v>0.5</v>
-      </c>
-      <c r="AZ5">
-        <v>0.5</v>
+      <c r="X5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AP5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AQ5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AR5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AS5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AT5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AV5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AW5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AX5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AY5" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AZ5" s="2">
+        <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1006,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1026,7 +1034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1044,6 +1052,17 @@
       </c>
       <c r="G8">
         <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="L9">
+        <v>1E-8</v>
       </c>
     </row>
   </sheetData>
@@ -1053,18 +1072,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794004A-4C7C-4E94-81C3-7E7CA0B5D399}">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3:AV3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1078,73 +1097,139 @@
         <v>2018</v>
       </c>
       <c r="E1">
+        <v>2018.5</v>
+      </c>
+      <c r="F1">
         <v>2019</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>2019.5</v>
+      </c>
+      <c r="H1">
         <v>2020</v>
       </c>
-      <c r="G1">
+      <c r="I1">
+        <v>2020.5</v>
+      </c>
+      <c r="J1">
         <v>2021</v>
       </c>
-      <c r="H1">
+      <c r="K1">
+        <v>2021.5</v>
+      </c>
+      <c r="L1">
         <v>2022</v>
       </c>
-      <c r="I1">
+      <c r="M1">
+        <v>2022.5</v>
+      </c>
+      <c r="N1">
         <v>2023</v>
       </c>
-      <c r="J1">
+      <c r="O1">
+        <v>2023.5</v>
+      </c>
+      <c r="P1">
         <v>2024</v>
       </c>
-      <c r="K1">
+      <c r="Q1">
+        <v>2024.5</v>
+      </c>
+      <c r="R1">
         <v>2025</v>
       </c>
-      <c r="L1">
+      <c r="S1">
+        <v>2025.5</v>
+      </c>
+      <c r="T1">
         <v>2026</v>
       </c>
-      <c r="M1">
+      <c r="U1">
+        <v>2026.5</v>
+      </c>
+      <c r="V1">
         <v>2027</v>
       </c>
-      <c r="N1">
+      <c r="W1">
+        <v>2027.5</v>
+      </c>
+      <c r="X1">
         <v>2028</v>
       </c>
-      <c r="O1">
+      <c r="Y1">
+        <v>2028.5</v>
+      </c>
+      <c r="Z1">
         <v>2029</v>
       </c>
-      <c r="P1">
+      <c r="AA1">
+        <v>2029.5</v>
+      </c>
+      <c r="AB1">
         <v>2030</v>
       </c>
-      <c r="Q1">
+      <c r="AC1">
+        <v>2030.5</v>
+      </c>
+      <c r="AD1">
         <v>2031</v>
       </c>
-      <c r="R1">
+      <c r="AE1">
+        <v>2031.5</v>
+      </c>
+      <c r="AF1">
         <v>2032</v>
       </c>
-      <c r="S1">
+      <c r="AG1">
+        <v>2032.5</v>
+      </c>
+      <c r="AH1">
         <v>2033</v>
       </c>
-      <c r="T1">
+      <c r="AI1">
+        <v>2033.5</v>
+      </c>
+      <c r="AJ1">
         <v>2034</v>
       </c>
-      <c r="U1">
+      <c r="AK1">
+        <v>2034.5</v>
+      </c>
+      <c r="AL1">
         <v>2035</v>
       </c>
-      <c r="V1">
+      <c r="AM1">
+        <v>2035.5</v>
+      </c>
+      <c r="AN1">
         <v>2036</v>
       </c>
-      <c r="W1">
+      <c r="AO1">
+        <v>2036.5</v>
+      </c>
+      <c r="AP1">
         <v>2037</v>
       </c>
-      <c r="X1">
+      <c r="AQ1">
+        <v>2037.5</v>
+      </c>
+      <c r="AR1">
         <v>2038</v>
       </c>
-      <c r="Y1">
+      <c r="AS1">
+        <v>2038.5</v>
+      </c>
+      <c r="AT1">
         <v>2039</v>
       </c>
-      <c r="Z1">
+      <c r="AU1">
+        <v>2039.5</v>
+      </c>
+      <c r="AV1">
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1234,8 +1319,74 @@
       <c r="Z3">
         <v>1</v>
       </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>1</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1246,7 +1397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1257,7 +1408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1279,7 +1430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1307,12 +1458,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1533,15 +1681,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1566,10 +1718,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
upload files for new runs
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_2.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewgraham/Dropbox/ntd-model-sch/sch_simulation/data/Scenarios_8_3_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31B00D9-DC98-314A-8003-BDBDDB89DAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CB0250-2822-354C-8E4B-BA60D027EFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44020" windowHeight="20360" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
   <si>
     <t>Country/Region</t>
   </si>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
-  <dimension ref="A1:AZ9"/>
+  <dimension ref="A1:AZ8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="X4" s="2">
         <v>0.61299999999999999</v>
@@ -895,106 +895,19 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>50</v>
-      </c>
-      <c r="G5">
-        <v>65</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AK5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AN5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AO5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AP5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AQ5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AR5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AS5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AT5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AU5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AV5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AW5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AX5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AY5" s="2">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="AZ5" s="2">
-        <v>0.61299999999999999</v>
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.2">
@@ -1008,13 +921,13 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.2">
@@ -1025,46 +938,26 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>14</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="K9">
+      <c r="K8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="L9">
+      <c r="L8">
         <v>1E-8</v>
       </c>
     </row>
@@ -1461,21 +1354,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3B750AFB9343D42B939C6ACF084A84C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93cd09b7eadf1f96f07e4cafc6f5cdf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00318829-ac19-4fa6-afcb-83e1ad4ea23b" xmlns:ns3="5ffa21b6-e00b-4719-91c3-427b29c2b057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb8f100d907d4c7940a7c9646b5f1c73" ns2:_="" ns3:_="">
     <xsd:import namespace="00318829-ac19-4fa6-afcb-83e1ad4ea23b"/>
@@ -1692,24 +1570,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6E6D53-A4AA-4BF4-8C61-16B862AC0A51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1726,4 +1602,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>